<commit_message>
Modelo Relacional arreglado según SQL
</commit_message>
<xml_diff>
--- a/docs/Proyecto modelo relacional.xlsx
+++ b/docs/Proyecto modelo relacional.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Cardona\OneDrive\Documentos\Cuarto semestre\Sistemas Transaccionales\Proyecto\Iteración 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Cardona\OneDrive\Documentos\Cuarto semestre\Sistemas Transaccionales\Semana 9\Iteracion2AforoCCANDES\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62FADFA-1567-41DD-BA65-20FFEF471503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE77E05-2C3F-4D7F-944B-6CBF8D77569A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="56">
   <si>
     <t>nombre</t>
   </si>
@@ -39,9 +39,6 @@
     <t>NN</t>
   </si>
   <si>
-    <t>FK</t>
-  </si>
-  <si>
     <t>FK,NN</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>idLector</t>
   </si>
   <si>
-    <t>fechaYHoraOp</t>
-  </si>
-  <si>
     <t>Visita</t>
   </si>
   <si>
@@ -105,21 +99,6 @@
     <t>telefono</t>
   </si>
   <si>
-    <t>nombreContacto</t>
-  </si>
-  <si>
-    <t>telefonoContacto</t>
-  </si>
-  <si>
-    <t>codigoQR</t>
-  </si>
-  <si>
-    <t>horarioDisponible</t>
-  </si>
-  <si>
-    <t>tipoVisitante</t>
-  </si>
-  <si>
     <t>tipoEspacio</t>
   </si>
   <si>
@@ -132,9 +111,6 @@
     <t>nombreEmpresa</t>
   </si>
   <si>
-    <t>tiopOp</t>
-  </si>
-  <si>
     <t>Parqueadero</t>
   </si>
   <si>
@@ -151,6 +127,72 @@
   </si>
   <si>
     <t xml:space="preserve"> NN</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>TimeStamp</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>PK, NN</t>
+  </si>
+  <si>
+    <t>FK, NN</t>
+  </si>
+  <si>
+    <t>Varchar2</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Id_Parqueadero</t>
+  </si>
+  <si>
+    <t>Id_Local</t>
+  </si>
+  <si>
+    <t>Id_Espacio</t>
+  </si>
+  <si>
+    <t>Id_Baño</t>
+  </si>
+  <si>
+    <t>fechaYHora_Op</t>
+  </si>
+  <si>
+    <t>tipo_Op</t>
+  </si>
+  <si>
+    <t>horaFin_Op</t>
+  </si>
+  <si>
+    <t>PK,FK,NN</t>
+  </si>
+  <si>
+    <t>nombre_Contacto</t>
+  </si>
+  <si>
+    <t>NN,CK('Empleado','Vigilancia','Aseo','Mantenimiento','Clientes','Domiciliarios','Administrador_centro','Administrador_local')</t>
+  </si>
+  <si>
+    <t>tipo_Visitante</t>
+  </si>
+  <si>
+    <t>codigo_QR</t>
+  </si>
+  <si>
+    <t>telefono_Contacto</t>
+  </si>
+  <si>
+    <t>horario_Disponible</t>
+  </si>
+  <si>
+    <t>VarChar2</t>
   </si>
 </sst>
 </file>
@@ -250,7 +292,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -270,6 +312,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -554,54 +606,54 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="B1:P38"/>
+  <dimension ref="B1:Q38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="2"/>
-    <col min="16" max="16" width="18.5703125" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="8.7109375" style="2"/>
+    <col min="2" max="3" width="18.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="19" style="2" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" style="2"/>
+    <col min="17" max="17" width="18.5703125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -611,413 +663,441 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="P8" s="6"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>16</v>
+      <c r="G18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>22</v>
+      <c r="H30" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="H31" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>2</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>3</v>
@@ -1043,29 +1123,49 @@
       <c r="J35" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L35" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
+      <c r="K35" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="L36" s="6"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I36" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="9"/>
+      <c r="E38" s="8" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>